<commit_message>
fixes #974 - add value URI for subject in spreadsheet loader
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods_new_file/demo_mods_new_file.xlsx
+++ b/spec/fixtures/files/demo_mods_new_file/demo_mods_new_file.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="160">
   <si>
     <t>What is your name?</t>
   </si>
@@ -347,9 +347,6 @@
     <t xml:space="preserve">Donated by Citywide Educational Coalition. </t>
   </si>
   <si>
-    <t>African American students -- Massachusetts -- Boston</t>
-  </si>
-  <si>
     <t>lcsh</t>
   </si>
   <si>
@@ -504,6 +501,12 @@
   </si>
   <si>
     <t>Language 1</t>
+  </si>
+  <si>
+    <t>African American students -- Massachusetts -- Boston | Value URI</t>
+  </si>
+  <si>
+    <t>African Americans -- Education -- Massachusetts -- Boston | Value URI</t>
   </si>
 </sst>
 </file>
@@ -867,7 +870,7 @@
   <dimension ref="A1:CJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2"/>
+      <selection activeCell="BK2" sqref="BK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1045,7 @@
         <v>52</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BC1" s="1" t="s">
         <v>53</v>
@@ -1105,28 +1108,28 @@
         <v>72</v>
       </c>
       <c r="BW1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="BX1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="BZ1" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="CA1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CB1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>73</v>
@@ -1180,7 +1183,7 @@
         <v>87</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
@@ -1193,7 +1196,7 @@
         <v>89</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>90</v>
@@ -1262,7 +1265,7 @@
         <v>102</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC2" s="1" t="s">
         <v>103</v>
@@ -1277,28 +1280,28 @@
       </c>
       <c r="BH2" s="1"/>
       <c r="BI2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BJ2" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="BK2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BL2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BN2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BN2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BO2" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="BP2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BQ2" s="1"/>
       <c r="BR2" s="1"/>
@@ -1317,7 +1320,7 @@
       </c>
       <c r="BZ2" s="1"/>
       <c r="CA2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="CB2" s="1" t="s">
         <v>86</v>
@@ -1330,19 +1333,19 @@
         <v>84</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="CG2" s="1" t="s">
         <v>81</v>
       </c>
       <c r="CH2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CI2" s="4">
         <v>42170.508518518516</v>
       </c>
       <c r="CJ2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:88" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1350,10 +1353,10 @@
         <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>82</v>
@@ -1373,11 +1376,11 @@
         <v>87</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>86</v>
@@ -1409,13 +1412,13 @@
         <v>92</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AM3" s="3" t="s">
         <v>94</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AO3" s="2"/>
       <c r="AP3" s="1"/>
@@ -1435,16 +1438,16 @@
         <v>100</v>
       </c>
       <c r="AZ3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BA3" s="1" t="s">
         <v>102</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BD3" s="2"/>
       <c r="BE3" s="2"/>
@@ -1456,28 +1459,28 @@
       </c>
       <c r="BH3" s="2"/>
       <c r="BI3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BJ3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BK3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BL3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BN3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO3" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BL3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BM3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BN3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BO3" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="BP3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
@@ -1486,7 +1489,7 @@
       <c r="BU3" s="1"/>
       <c r="BV3" s="1"/>
       <c r="BW3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BX3" s="1" t="s">
         <v>86</v>
@@ -1496,29 +1499,29 @@
       </c>
       <c r="BZ3" s="1"/>
       <c r="CA3" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="CB3" s="1"/>
       <c r="CC3" s="1" t="s">
         <v>87</v>
       </c>
       <c r="CE3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CF3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="CG3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CH3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CI3" s="8">
         <v>42285.597905092596</v>
       </c>
       <c r="CJ3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:88" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1526,17 +1529,17 @@
         <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1552,11 +1555,11 @@
         <v>87</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>86</v>
@@ -1588,13 +1591,13 @@
         <v>92</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM4" s="3" t="s">
         <v>94</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AO4" s="2"/>
       <c r="AP4" s="2"/>
@@ -1614,16 +1617,16 @@
         <v>100</v>
       </c>
       <c r="AZ4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="BA4" s="1" t="s">
         <v>102</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="BD4" s="2"/>
       <c r="BE4" s="2"/>
@@ -1657,22 +1660,22 @@
       <c r="CC4" s="1"/>
       <c r="CD4" s="6"/>
       <c r="CE4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="CF4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="CG4" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="CH4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CI4" s="8">
         <v>42285.606759259259</v>
       </c>
       <c r="CJ4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:88" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1680,24 +1683,24 @@
         <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>86</v>
@@ -1706,13 +1709,13 @@
         <v>89</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>86</v>
@@ -1744,13 +1747,13 @@
         <v>92</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM5" s="3" t="s">
         <v>94</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AO5" s="2"/>
       <c r="AP5" s="2"/>
@@ -1770,16 +1773,16 @@
         <v>100</v>
       </c>
       <c r="AZ5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BA5" s="1" t="s">
         <v>102</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BD5" s="2"/>
       <c r="BE5" s="2"/>
@@ -1791,28 +1794,28 @@
       </c>
       <c r="BH5" s="2"/>
       <c r="BI5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BJ5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BK5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BL5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BN5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BL5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BM5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BN5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BO5" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="BP5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BQ5" s="1"/>
       <c r="BR5" s="1"/>
@@ -1821,7 +1824,7 @@
       <c r="BU5" s="1"/>
       <c r="BV5" s="1"/>
       <c r="BW5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BX5" s="1" t="s">
         <v>86</v>
@@ -1831,7 +1834,7 @@
       </c>
       <c r="BZ5" s="1"/>
       <c r="CA5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="CB5" s="1" t="s">
         <v>86</v>
@@ -1840,22 +1843,22 @@
         <v>89</v>
       </c>
       <c r="CE5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="CF5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="CG5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CH5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CI5" s="8">
         <v>42285.616435185184</v>
       </c>
       <c r="CJ5" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>